<commit_message>
need tuning for negara handling, the 3w done
</commit_message>
<xml_diff>
--- a/whowherewhen/whowhenwhere_test_result_bencana.xlsx
+++ b/whowherewhen/whowhenwhere_test_result_bencana.xlsx
@@ -551,8 +551,10 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="n">
-        <v>0</v>
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Noor Jannah, Ungaran, BMKG Stasiun Meteorologi Ahmad Yani</t>
+        </is>
       </c>
       <c r="B2" t="n">
         <v>0</v>
@@ -665,8 +667,10 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="n">
-        <v>0</v>
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Koordinator Sekretariat Bawaslu, Hisyam Wahyu Aditya, Panwascam, Hisyam, Banjir</t>
+        </is>
       </c>
       <c r="B3" t="n">
         <v>0</v>
@@ -780,8 +784,10 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="n">
-        <v>0</v>
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Hardi Ariyanto, Hardi Aryanto, Cabang Bandara Internasional Jenderal Ahmad Yani, Satuan Korps Brimob Polda, Hadi, Darat Ahmad Yani</t>
+        </is>
       </c>
       <c r="B4" t="n">
         <v>0</v>
@@ -905,8 +911,10 @@
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="n">
-        <v>0</v>
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>BPBD, Peringatan Dini Tsunami BMKG Dr Daryono, Didik Wahyudi, Gindosari, Gempa, Australia, Daryono, BMKG, Populer</t>
+        </is>
       </c>
       <c r="B5" t="n">
         <v>0</v>
@@ -1022,8 +1030,10 @@
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="n">
-        <v>0</v>
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Pura Luhur Uluwatu Pura Luhur Uluwatu, Museum, Ganesa, Dinas Pariwisata, Ancak Saji, Sang Hyang Widhi Wasa, Penasaran, Pelelindon, Megawati Soekarno Putri, Dinas Kebudayaan, Nista Mandala, Kerta Gosa, Bhiksu, Trimurti, Anom, Pura Besakih, Tari Kecak, Gunung Mas, Dwarapala, Semarapura, Tenganan Pegringsingan, Pura Tanah Lot, India, Bandara Ngurah Rai, Madya Mandala, Swarga, Saren Agung, Pura Yeh Pulu, Catur Karya, Wisatawan, Dajan Peken, Tumbu, Garuda Wisnu Kencana, Pura Tirta Empul, Pasar Seni, Wisata Air Tirta, Soekarno, Monumen Bajra Sandi, Penglipuran, Bentar, Pan Brayut, Shri I Gusti Ngrh, Sukmawati Sukarno, Tirta Empul, Pura Uluwatu, Kamasan, Ni Dyah Tantri, Nah, Ratu Tribhuwana Tunggadewi, Belanda, Sanur Kauh, Museum Blanco Renaissance Musuem Blanco Renaissance, Panjer, Beraban, Monumen Bajra Sandhi, Suci Ageng, Punggawa, Bale Kembar, Tri Mandala, Brahma, Pulau Seribu Pura, Wisnu, Wisata Tirta, Ir, Piodalan, Curt Grundler, Pura Kiduling Kreteg, Loto Ang, Sansekerta, Besakih, Tanah Lot, Bersejarah, Palelintangan, Campuhan, Blahbatuh, Pura Penataran Sasih Pura Penataran Sasih, Museum Soekarno, Phalguna, Tampaksiring, Tandekan, Madeg, Tegallinggah, Anak Agung Agung Anglurah Ketut, Paviliun, Dangin, Pantai Dreamland, Pejeng, Pura, Puputan, Goa, Jl, Ababi, Prasasti Blanjong, Jadi</t>
+        </is>
       </c>
       <c r="B6" t="n">
         <v>0</v>
@@ -1385,8 +1395,10 @@
       </c>
     </row>
     <row r="7">
-      <c r="A7" t="n">
-        <v>0</v>
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Tangkap Ikan, Kasat Pol Air, ABK, Tabroni, AKP I Putu Raka Wirama, G20, Abdul Azis, Agus, Yuda, Akmal, PPN Pengambengan, Pengambengan, Kepala Cabang PT, Nahkoda Kapal, Raka, Pelabuhan Benoa, Muliyono</t>
+        </is>
       </c>
       <c r="B7" t="n">
         <v>0</v>
@@ -1502,8 +1514,10 @@
       </c>
     </row>
     <row r="8">
-      <c r="A8" t="n">
-        <v>0</v>
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Badan Meteorologi, Klimatologi, Bujur, Gempa, BMKG</t>
+        </is>
       </c>
       <c r="B8" t="n">
         <v>0</v>
@@ -1611,8 +1625,10 @@
       </c>
     </row>
     <row r="9">
-      <c r="A9" t="n">
-        <v>0</v>
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Tatar, Amrullah, Labuhan, Sekokang KSB</t>
+        </is>
       </c>
       <c r="B9" t="n">
         <v>0</v>
@@ -1727,8 +1743,10 @@
       </c>
     </row>
     <row r="10">
-      <c r="A10" t="n">
-        <v>0</v>
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Pantauan, Dani, Jari, Gunung Semeru</t>
+        </is>
       </c>
       <c r="B10" t="n">
         <v>0</v>
@@ -1844,8 +1862,10 @@
       </c>
     </row>
     <row r="11">
-      <c r="A11" t="n">
-        <v>0</v>
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Aldi, Warga, Aldi Tri Pamungkas, Pasar, Kementerian PUPR</t>
+        </is>
       </c>
       <c r="B11" t="n">
         <v>0</v>
@@ -1962,8 +1982,10 @@
       </c>
     </row>
     <row r="12">
-      <c r="A12" t="n">
-        <v>0</v>
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>NasDem Ahmad Ali, Pak Jokowi, Djarot, Menhut, Presiden Jokowi, NasDem, Mentan, PDIP, DPP Taruna Merah Putih, Bappenas, PDI Perjuangan, Jokowi, DPP PDIP Djarot Saiful Hidayat, Kementan, Ali, Djarot Saiful Hidayat</t>
+        </is>
       </c>
       <c r="B12" t="n">
         <v>0</v>
@@ -2117,8 +2139,10 @@
       </c>
     </row>
     <row r="13">
-      <c r="A13" t="n">
-        <v>0</v>
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>BPBD, DLH, Pelaksana BPBD, Sapri, Amiruddin, Baru, Fadli, Caddi, Pantai, Kepala Dinas Lingkungan Hidup, Nisombalia, TPA</t>
+        </is>
       </c>
       <c r="B13" t="n">
         <v>0</v>
@@ -2253,8 +2277,10 @@
       </c>
     </row>
     <row r="14">
-      <c r="A14" t="n">
-        <v>0</v>
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Dwikorita, Malut, Indonesia, NTT, BMKG, Kepala BMKG Dwikorita, NTB</t>
+        </is>
       </c>
       <c r="B14" t="n">
         <v>0</v>
@@ -2369,8 +2395,10 @@
       </c>
     </row>
     <row r="15">
-      <c r="A15" t="n">
-        <v>0</v>
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Mampang Prapatan, Penyelamatan, Arief, Nike, Moch Arief</t>
+        </is>
       </c>
       <c r="B15" t="n">
         <v>0</v>
@@ -2483,8 +2511,10 @@
       </c>
     </row>
     <row r="16">
-      <c r="A16" t="n">
-        <v>0</v>
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>Jabodetabek, BRIN Erma Yulihastin, Benyamin, Erma, BMKG, Benyamin Davnie</t>
+        </is>
       </c>
       <c r="B16" t="n">
         <v>0</v>
@@ -2610,8 +2640,10 @@
       </c>
     </row>
     <row r="17">
-      <c r="A17" t="n">
-        <v>0</v>
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>Andi, Peneliti, Riset Antariksa BRIN, KawanBRIN, Riset Antariksa BRIN Andi</t>
+        </is>
       </c>
       <c r="B17" t="n">
         <v>0</v>
@@ -2736,8 +2768,10 @@
       </c>
     </row>
     <row r="18">
-      <c r="A18" t="n">
-        <v>0</v>
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>Antara, Kali Kuning, Kapanewon, Kuntoro</t>
+        </is>
       </c>
       <c r="B18" t="n">
         <v>0</v>
@@ -2849,8 +2883,10 @@
       </c>
     </row>
     <row r="19">
-      <c r="A19" t="n">
-        <v>0</v>
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>Herman, Herman Suherman, Kejari</t>
+        </is>
       </c>
       <c r="B19" t="n">
         <v>0</v>
@@ -2898,12 +2934,12 @@
       </c>
       <c r="N19" t="inlineStr">
         <is>
-          <t>cianjur</t>
+          <t>-</t>
         </is>
       </c>
       <c r="O19" t="inlineStr">
         <is>
-          <t>jawa barat</t>
+          <t>-</t>
         </is>
       </c>
       <c r="P19" t="n">
@@ -2968,8 +3004,10 @@
       </c>
     </row>
     <row r="20">
-      <c r="A20" t="n">
-        <v>0</v>
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>Iya, BMKG, Nindi, Yakub</t>
+        </is>
       </c>
       <c r="B20" t="n">
         <v>0</v>
@@ -3087,8 +3125,10 @@
       </c>
     </row>
     <row r="21">
-      <c r="A21" t="n">
-        <v>0</v>
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>Jin, BTS Kim Namjoon, Yonhap, BIGHIT Music, Weverse, Harap, Jin BTS, Korea, J Hope, Yeoncheon, BIGHIT, BTS</t>
+        </is>
       </c>
       <c r="B21" t="n">
         <v>0</v>
@@ -3227,8 +3267,10 @@
       </c>
     </row>
     <row r="22">
-      <c r="A22" t="n">
-        <v>0</v>
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>Ganis Dyah Limaran, Sekretaris BPBD, Tadi, Daya, Mujito, Pucung, Gubuk Mas, MMI, BMKG</t>
+        </is>
       </c>
       <c r="B22" t="n">
         <v>0</v>
@@ -3351,8 +3393,10 @@
       </c>
     </row>
     <row r="23">
-      <c r="A23" t="n">
-        <v>0</v>
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>Klimatologi, ASDP, Ira Puspadewi, Nataru, Gilimanuk, Over Dimension, Ira, Sumatera, Penumpang Kapal Selama Nataru, ODOL</t>
+        </is>
       </c>
       <c r="B23" t="n">
         <v>0</v>
@@ -3400,12 +3444,12 @@
       </c>
       <c r="N23" t="inlineStr">
         <is>
-          <t>banyuwangi</t>
+          <t>ketapang</t>
         </is>
       </c>
       <c r="O23" t="inlineStr">
         <is>
-          <t>jawa timur</t>
+          <t>kalimantan barat</t>
         </is>
       </c>
       <c r="P23" t="n">
@@ -3550,8 +3594,10 @@
       </c>
     </row>
     <row r="24">
-      <c r="A24" t="n">
-        <v>0</v>
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>Sungai Silugonggo, Marzuki, Kerugian, Warga</t>
+        </is>
       </c>
       <c r="B24" t="n">
         <v>0</v>
@@ -3674,8 +3720,10 @@
       </c>
     </row>
     <row r="25">
-      <c r="A25" t="n">
-        <v>0</v>
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>Sulis, Bhabinkamtibmas, Sulistiono, Terminal, Susanto, Aiptu Susanto, Wetan, RA Agil Kusumadya</t>
+        </is>
       </c>
       <c r="B25" t="n">
         <v>0</v>
@@ -3793,8 +3841,10 @@
       </c>
     </row>
     <row r="26">
-      <c r="A26" t="n">
-        <v>0</v>
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>Fitriani, Suwandi, IGD RS Pelamonia, Fitriani Sudirman, DLHD, Dinas Lingkungan Hidup, Pomanto, RS TK Pelamonia, Pandang Bripka Suwandhi, Pemkot, Danny, Kasi Humas Polsek</t>
+        </is>
       </c>
       <c r="B26" t="n">
         <v>0</v>
@@ -3915,8 +3965,10 @@
       </c>
     </row>
     <row r="27">
-      <c r="A27" t="n">
-        <v>0</v>
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>Amir, Pohon, Kakek Dg Gewa, Hasanuddin, Kakek, Dg Gewa, Korban, Keluruhan, SAR, Kadis Damkar</t>
+        </is>
       </c>
       <c r="B27" t="n">
         <v>0</v>
@@ -4032,8 +4084,10 @@
       </c>
     </row>
     <row r="28">
-      <c r="A28" t="n">
-        <v>0</v>
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>Heru Budi Hartono, Heru Budi, Pemprov DKI, Heru, Gubernur DKI, Waduk Pluit</t>
+        </is>
       </c>
       <c r="B28" t="n">
         <v>0</v>
@@ -4146,8 +4200,10 @@
       </c>
     </row>
     <row r="29">
-      <c r="A29" t="n">
-        <v>0</v>
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>Cecep Alamsyah, Korban, Kontributor, Teguh Rahayu, Kepala BMKG, BMKG</t>
+        </is>
       </c>
       <c r="B29" t="n">
         <v>0</v>
@@ -4278,8 +4334,10 @@
       </c>
     </row>
     <row r="30">
-      <c r="A30" t="n">
-        <v>0</v>
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>DKPP, Arifin, Kementerian Pertanian, Moh Arifin Soedjayana</t>
+        </is>
       </c>
       <c r="B30" t="n">
         <v>0</v>
@@ -4400,8 +4458,10 @@
       </c>
     </row>
     <row r="31">
-      <c r="A31" t="n">
-        <v>0</v>
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>Mario, RSU BRI Medika, Muhammad Teguh Budi Wibowo, Whatsapp, UPT Pemadam Kebakaran, Jembatan Suhat, Irfan, Suhat, Lama, PMI, M Irfan</t>
+        </is>
       </c>
       <c r="B31" t="n">
         <v>0</v>
@@ -4522,8 +4582,10 @@
       </c>
     </row>
     <row r="32">
-      <c r="A32" t="n">
-        <v>0</v>
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>Febby Rizky Pratama, BPBD, Samudra Pasifik, Febby, Indonesia, Rizky</t>
+        </is>
       </c>
       <c r="B32" t="n">
         <v>0</v>
@@ -4652,8 +4714,10 @@
       </c>
     </row>
     <row r="33">
-      <c r="A33" t="n">
-        <v>0</v>
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>Selengkapnya, Pengungsian, Dinas Sosial, Gubernur, Ganjar, Sungai Bremi, Ganjar Pranowo, Aula</t>
+        </is>
       </c>
       <c r="B33" t="n">
         <v>0</v>
@@ -4785,8 +4849,10 @@
       </c>
     </row>
     <row r="34">
-      <c r="A34" t="n">
-        <v>0</v>
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>Gatot, Antara, Pulogadung, Jl Pisangan Lama, Gatot Sulaiman, Jl DI Panjaitan, Gatot Sulaeman, Jl Jendral Ahmad Yani, Kasi Operasional Sudin Gulkarmat Jaktim, Asem Gede</t>
+        </is>
       </c>
       <c r="B34" t="n">
         <v>0</v>
@@ -4899,8 +4965,10 @@
       </c>
     </row>
     <row r="35">
-      <c r="A35" t="n">
-        <v>0</v>
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>Klimatologi, Erma Yulihastin, La Nina, Jabodetabek, BNPB Letjen TNI Suharyanto, Sunda, Kementerian Perhubungan, Menhub, TMC, BRIN, Erma, Squall Line, BNPB</t>
+        </is>
       </c>
       <c r="B35" t="n">
         <v>0</v>
@@ -5056,8 +5124,10 @@
       </c>
     </row>
     <row r="36">
-      <c r="A36" t="n">
-        <v>0</v>
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>Prakirawan BMKG, Benny Gumintar, Banjir, Benny, BMKG</t>
+        </is>
       </c>
       <c r="B36" t="n">
         <v>0</v>
@@ -5178,8 +5248,10 @@
       </c>
     </row>
     <row r="37">
-      <c r="A37" t="n">
-        <v>0</v>
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>Klimatologi, Anton Sugiarto, Mukomuko, Enim, Anton, Megathrust, Subduksi, BMKG, Komering</t>
+        </is>
       </c>
       <c r="B37" t="n">
         <v>0</v>
@@ -5304,8 +5376,10 @@
       </c>
     </row>
     <row r="38">
-      <c r="A38" t="n">
-        <v>0</v>
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>Kebon Jeruk, Sardi</t>
+        </is>
       </c>
       <c r="B38" t="n">
         <v>0</v>
@@ -5411,8 +5485,10 @@
       </c>
     </row>
     <row r="39">
-      <c r="A39" t="n">
-        <v>0</v>
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>Maria Theresia Ekawati Rahayu, Pemkot</t>
+        </is>
       </c>
       <c r="B39" t="n">
         <v>0</v>
@@ -5533,8 +5609,10 @@
       </c>
     </row>
     <row r="40">
-      <c r="A40" t="n">
-        <v>0</v>
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>BPBD, Ariadi, Ariadi Pribadi</t>
+        </is>
       </c>
       <c r="B40" t="n">
         <v>0</v>
@@ -5648,8 +5726,10 @@
       </c>
     </row>
     <row r="41">
-      <c r="A41" t="n">
-        <v>0</v>
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>DLH, Sapri, Amiruddin, Caddi, Pantai, Kepala Dinas Lingkungan Hidup, Nisombalia, Kepala, TPA</t>
+        </is>
       </c>
       <c r="B41" t="n">
         <v>0</v>
@@ -5765,8 +5845,10 @@
       </c>
     </row>
     <row r="42">
-      <c r="A42" t="n">
-        <v>0</v>
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>BMKG Juanda</t>
+        </is>
       </c>
       <c r="B42" t="n">
         <v>0</v>
@@ -5884,8 +5966,10 @@
       </c>
     </row>
     <row r="43">
-      <c r="A43" t="n">
-        <v>0</v>
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>Pemkab, Cecep</t>
+        </is>
       </c>
       <c r="B43" t="n">
         <v>0</v>
@@ -5999,8 +6083,10 @@
       </c>
     </row>
     <row r="44">
-      <c r="A44" t="n">
-        <v>0</v>
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>Jelambar, Petamburan, Sugimanto</t>
+        </is>
       </c>
       <c r="B44" t="n">
         <v>0</v>
@@ -6121,8 +6207,10 @@
       </c>
     </row>
     <row r="45">
-      <c r="A45" t="n">
-        <v>0</v>
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>Pantai Marina, Pantauan, Kompol Dicky Hermansyah, Mbak Ita</t>
+        </is>
       </c>
       <c r="B45" t="n">
         <v>0</v>
@@ -6243,8 +6331,10 @@
       </c>
     </row>
     <row r="46">
-      <c r="A46" t="n">
-        <v>0</v>
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>Api, Iptu Agus Winarno, Gigih, Agus, Kasi Humas Polresta</t>
+        </is>
       </c>
       <c r="B46" t="n">
         <v>0</v>
@@ -6368,8 +6458,10 @@
       </c>
     </row>
     <row r="47">
-      <c r="A47" t="n">
-        <v>0</v>
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>Longsor, Poros, Ikhsan Parawansa, Ikhsan</t>
+        </is>
       </c>
       <c r="B47" t="n">
         <v>0</v>
@@ -6489,8 +6581,10 @@
       </c>
     </row>
     <row r="48">
-      <c r="A48" t="n">
-        <v>0</v>
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>Arif N, Ungaran, BMKG Stasiun Meteorologi Ahmad Yani</t>
+        </is>
       </c>
       <c r="B48" t="n">
         <v>0</v>
@@ -6603,8 +6697,10 @@
       </c>
     </row>
     <row r="49">
-      <c r="A49" t="n">
-        <v>0</v>
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>Dinas Koperasi UMKM, BPBD, Kepolisian, Damkar, Polisi, Pasar, C, Iwan Ridwan, Bagian Operasi Polresta, Kompol Shohet, TNI, Blok C Pasar, Iwan</t>
+        </is>
       </c>
       <c r="B49" t="n">
         <v>0</v>
@@ -6731,8 +6827,10 @@
       </c>
     </row>
     <row r="50">
-      <c r="A50" t="n">
-        <v>0</v>
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>Pedukuhan Cegokan, Sugito, Adib, Cinomati, Nataru, Kalurahan Wonolelo, Jalur Cinomati, Google Maps, FPRB, Cegokan, Kapanewon, Dukuh Cegokan Sugito</t>
+        </is>
       </c>
       <c r="B50" t="n">
         <v>0</v>
@@ -6865,8 +6963,10 @@
       </c>
     </row>
     <row r="51">
-      <c r="A51" t="n">
-        <v>0</v>
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>Bupati, Ajudan Bupati, BMKG Stasiun Geofisika, Teguh Rahayu, Jeje, AKP Luhut Sitorus, Jeje Wiradinta, Jeje Wiradinata, Islah, Aswin, Eurasia, Klimatologi, Kombes Pol Aswin Sipayung, Andi, Kasat Reskrim Polres, Satpol PP, Stasiun Geofisika, Al Jabbar, XEKRILE, Geng Motor XEKRILE, Mapolrestabes, Rahayu, Kapolrestabes, Nandang Suhendar, Geng Motor, BMKG Stasiun, Masjid, BMKG, Agus, Luhut</t>
+        </is>
       </c>
       <c r="B51" t="n">
         <v>0</v>
@@ -7054,8 +7154,10 @@
       </c>
     </row>
     <row r="52">
-      <c r="A52" t="n">
-        <v>0</v>
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>Heru Budi Hartono, Mampang Prapatan, Damkar, Kepala BNPB, Heru Budi, Heru, Gubernur DKI, BNPB</t>
+        </is>
       </c>
       <c r="B52" t="n">
         <v>0</v>
@@ -7166,8 +7268,10 @@
       </c>
     </row>
     <row r="53">
-      <c r="A53" t="n">
-        <v>0</v>
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>Ridwan Muarif, Jl, Pelaksana Tugas</t>
+        </is>
       </c>
       <c r="B53" t="n">
         <v>0</v>
@@ -7278,8 +7382,10 @@
       </c>
     </row>
     <row r="54">
-      <c r="A54" t="n">
-        <v>0</v>
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>Rawa Cupang, Haji Garie, TMC Polda, JL, DKI, Tol JORR, Kec, Jl, Instagram TMC Polda, Penganten Ali</t>
+        </is>
       </c>
       <c r="B54" t="n">
         <v>0</v>
@@ -7401,8 +7507,10 @@
       </c>
     </row>
     <row r="55">
-      <c r="A55" t="n">
-        <v>0</v>
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>Titi, Yopi, Kapolsek Matan Hilir, Ipda Meinardus</t>
+        </is>
       </c>
       <c r="B55" t="n">
         <v>0</v>
@@ -7508,8 +7616,10 @@
       </c>
     </row>
     <row r="56">
-      <c r="A56" t="n">
-        <v>0</v>
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>Camat, Pomanto, Biringkanaya, Danny</t>
+        </is>
       </c>
       <c r="B56" t="n">
         <v>0</v>
@@ -7634,8 +7744,10 @@
       </c>
     </row>
     <row r="57">
-      <c r="A57" t="n">
-        <v>0</v>
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>BPBD, Laut, Ida Bagus Ketut Arimbawa, Arimbawa, BMKG, Badan Penanggulangan</t>
+        </is>
       </c>
       <c r="B57" t="n">
         <v>0</v>
@@ -7753,8 +7865,10 @@
       </c>
     </row>
     <row r="58">
-      <c r="A58" t="n">
-        <v>0</v>
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>Eh</t>
+        </is>
       </c>
       <c r="B58" t="n">
         <v>0</v>
@@ -7877,8 +7991,10 @@
       </c>
     </row>
     <row r="59">
-      <c r="A59" t="n">
-        <v>0</v>
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>Pulau, Bupati, ASDP Cabang, Uluwatu, GiriPrasta, PengelolaGWK, Gilimanuk, KTT G20, Pantai, Direktur Operasional GWK Stefanus Yonathan Astayasa</t>
+        </is>
       </c>
       <c r="B59" t="n">
         <v>0</v>
@@ -8001,8 +8117,10 @@
       </c>
     </row>
     <row r="60">
-      <c r="A60" t="n">
-        <v>0</v>
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>BMKG, Gempa</t>
+        </is>
       </c>
       <c r="B60" t="n">
         <v>0</v>
@@ -8109,8 +8227,10 @@
       </c>
     </row>
     <row r="61">
-      <c r="A61" t="n">
-        <v>0</v>
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>Said, BPBD, Erma Yulihastin, Jabodetabek, Pemkab, Baru, Twitternya, Erma</t>
+        </is>
       </c>
       <c r="B61" t="n">
         <v>0</v>
@@ -8250,8 +8370,10 @@
       </c>
     </row>
     <row r="62">
-      <c r="A62" t="n">
-        <v>0</v>
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>Gede, Laut, Perairan Kepulauan Kangean, Madura, Sutarno, Perairan, Masalembo, Bawean</t>
+        </is>
       </c>
       <c r="B62" t="n">
         <v>0</v>
@@ -8387,8 +8509,10 @@
       </c>
     </row>
     <row r="63">
-      <c r="A63" t="n">
-        <v>0</v>
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>Sastrawan, Pelaksanaan Transportasi Darat, I Nyoman Sastrawan, BPTD, Korsatpel, Nasional, Pelabuhan Gilimanuk</t>
+        </is>
       </c>
       <c r="B63" t="n">
         <v>0</v>
@@ -8504,8 +8628,10 @@
       </c>
     </row>
     <row r="64">
-      <c r="A64" t="n">
-        <v>0</v>
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>Nanti, Damkar, Hari, Pulo, Penyelamatan, Surono, Ridwan, Sudin Sosial, Melayu, Rusun, Pemkot, Inspeksi</t>
+        </is>
       </c>
       <c r="B64" t="n">
         <v>0</v>
@@ -8650,8 +8776,10 @@
       </c>
     </row>
     <row r="65">
-      <c r="A65" t="n">
-        <v>0</v>
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>G20, Indonesia, Panembahan Al Nahyan Nasution, Jokowi, Nahyan</t>
+        </is>
       </c>
       <c r="B65" t="n">
         <v>0</v>
@@ -8781,8 +8909,10 @@
       </c>
     </row>
     <row r="66">
-      <c r="A66" t="n">
-        <v>0</v>
+      <c r="A66" t="inlineStr">
+        <is>
+          <t>BMKG, Setiawan</t>
+        </is>
       </c>
       <c r="B66" t="n">
         <v>0</v>
@@ -8888,8 +9018,10 @@
       </c>
     </row>
     <row r="67">
-      <c r="A67" t="n">
-        <v>0</v>
+      <c r="A67" t="inlineStr">
+        <is>
+          <t>Badan Meteorologi, Klimatologi, Laut, Kaca, Gempa, Lapisan Bumi, BMKG</t>
+        </is>
       </c>
       <c r="B67" t="n">
         <v>0</v>
@@ -8932,12 +9064,12 @@
       </c>
       <c r="M67" t="inlineStr">
         <is>
-          <t>sumbawa</t>
+          <t>-</t>
         </is>
       </c>
       <c r="N67" t="inlineStr">
         <is>
-          <t>sumbawa</t>
+          <t>lombok utara</t>
         </is>
       </c>
       <c r="O67" t="inlineStr">
@@ -9015,8 +9147,10 @@
       </c>
     </row>
     <row r="68">
-      <c r="A68" t="n">
-        <v>0</v>
+      <c r="A68" t="inlineStr">
+        <is>
+          <t>BPBD, Martinus Budi Prasetya, Yitno, Bumirejo, RSUD, Budi</t>
+        </is>
       </c>
       <c r="B68" t="n">
         <v>0</v>
@@ -9126,8 +9260,10 @@
       </c>
     </row>
     <row r="69">
-      <c r="A69" t="n">
-        <v>0</v>
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>Brantas Abipraya Miftakhul Anas, PLTB, Terpanjang, Presiden Jokowi, PT Hutama Karya, Khofifah Indar Parawansa, Basuki, BUMN, Sungai Semantok, Tjahjo, Plt Bupati, Menteri Pekerjaan Umum, Sugeng Rochadi, Sekretaris Perusahaan Hutama Karya Tjahjo Purnomo, Indonesia, Marhaen Djumadi, Anas, Jokowi, Menteri PUPR Basuki Hadimuljono, Pelaksana Pembangunan, Gubernur, Semantok, Kab</t>
+        </is>
       </c>
       <c r="B69" t="n">
         <v>0</v>
@@ -9279,8 +9415,10 @@
       </c>
     </row>
     <row r="70">
-      <c r="A70" t="n">
-        <v>0</v>
+      <c r="A70" t="inlineStr">
+        <is>
+          <t>Klimatologi, Halmahera, BMKG, Gempa</t>
+        </is>
       </c>
       <c r="B70" t="n">
         <v>0</v>
@@ -9393,8 +9531,10 @@
       </c>
     </row>
     <row r="71">
-      <c r="A71" t="n">
-        <v>0</v>
+      <c r="A71" t="inlineStr">
+        <is>
+          <t>Abdul Munir, Pasir, Pantai</t>
+        </is>
       </c>
       <c r="B71" t="n">
         <v>0</v>
@@ -9506,8 +9646,10 @@
       </c>
     </row>
     <row r="72">
-      <c r="A72" t="n">
-        <v>0</v>
+      <c r="A72" t="inlineStr">
+        <is>
+          <t>Klimatologi, BMKG</t>
+        </is>
       </c>
       <c r="B72" t="n">
         <v>0</v>
@@ -9611,8 +9753,10 @@
       </c>
     </row>
     <row r="73">
-      <c r="A73" t="n">
-        <v>0</v>
+      <c r="A73" t="inlineStr">
+        <is>
+          <t>BPBD, Hendy, Alhamdulillah, Kidul, Jompo, Satpol PP, Sigit Akbari, Sigit</t>
+        </is>
       </c>
       <c r="B73" t="n">
         <v>0</v>
@@ -9725,8 +9869,10 @@
       </c>
     </row>
     <row r="74">
-      <c r="A74" t="n">
-        <v>0</v>
+      <c r="A74" t="inlineStr">
+        <is>
+          <t>Mampang Prapatan, BMKG, Jl Kapten P Tendean, Gempa</t>
+        </is>
       </c>
       <c r="B74" t="n">
         <v>0</v>
@@ -9828,8 +9974,10 @@
       </c>
     </row>
     <row r="75">
-      <c r="A75" t="n">
-        <v>0</v>
+      <c r="A75" t="inlineStr">
+        <is>
+          <t>BMKG, Wilayah, Dinoyo</t>
+        </is>
       </c>
       <c r="B75" t="n">
         <v>0</v>
@@ -9935,8 +10083,10 @@
       </c>
     </row>
     <row r="76">
-      <c r="A76" t="n">
-        <v>0</v>
+      <c r="A76" t="inlineStr">
+        <is>
+          <t>Andarias, Kepala BPBD Tana Toraja Christian Batara Sakkung, Miallo, Dinsos, Sembako, Iptu Andarias Tonapa, Kapolsek, Turbinnya, Mangose</t>
+        </is>
       </c>
       <c r="B76" t="n">
         <v>0</v>
@@ -10056,8 +10206,10 @@
       </c>
     </row>
     <row r="77">
-      <c r="A77" t="n">
-        <v>0</v>
+      <c r="A77" t="inlineStr">
+        <is>
+          <t>Emas, Pelabuhan, Kepala Bea Cukai Pelabuhan, Anton Martin</t>
+        </is>
       </c>
       <c r="B77" t="n">
         <v>0</v>
@@ -10170,8 +10322,10 @@
       </c>
     </row>
     <row r="78">
-      <c r="A78" t="n">
-        <v>0</v>
+      <c r="A78" t="inlineStr">
+        <is>
+          <t>Golkar, Yellow Clinic, Dwi Hartanto, Airlangga Hartarto, Presiden Joko Widodo, Yellow Clinic J Dwihartanto, RSUD Sayang, Dwi</t>
+        </is>
       </c>
       <c r="B78" t="n">
         <v>0</v>
@@ -10318,8 +10472,10 @@
       </c>
     </row>
     <row r="79">
-      <c r="A79" t="n">
-        <v>0</v>
+      <c r="A79" t="inlineStr">
+        <is>
+          <t>Prakirawan BMKG, Dyah, BMKG, Ganis Dyah</t>
+        </is>
       </c>
       <c r="B79" t="n">
         <v>0</v>
@@ -10433,8 +10589,10 @@
       </c>
     </row>
     <row r="80">
-      <c r="A80" t="n">
-        <v>0</v>
+      <c r="A80" t="inlineStr">
+        <is>
+          <t>Logistik BPBD Tangsel M Faridzal Gumay, Tol Alam, Gumay, Hujan, Tim BPBD Tangsel</t>
+        </is>
       </c>
       <c r="B80" t="n">
         <v>0</v>
@@ -10540,8 +10698,10 @@
       </c>
     </row>
     <row r="81">
-      <c r="A81" t="n">
-        <v>0</v>
+      <c r="A81" t="inlineStr">
+        <is>
+          <t>Sentral, B New, Ichsan, Energi Listrik, Dinas Pemadam Kebakaran, Wali, New, Fajrin, Sri, Danny Pomanto, PD Pasar, Karebosi, Ichsan Abduh Hussein, Direktur Utama Perumda Pasar, Mall, Pasar Sentral, Pengelolaan Sampah, Kepala Dinas Pemadam Kebakaran, Hasanuddin, Direktur PD Pasar, Abduh Hussein</t>
+        </is>
       </c>
       <c r="B81" t="n">
         <v>0</v>
@@ -10708,8 +10868,10 @@
       </c>
     </row>
     <row r="82">
-      <c r="A82" t="n">
-        <v>0</v>
+      <c r="A82" t="inlineStr">
+        <is>
+          <t>Direktur Lembaga Kajian Politik Nusakom Pratama Ari Junaedi, Wakil Wali, Dewan Perwakilan Rakyat Derah, TNI AU, Consulting Arif Nurul Imam, Imam, Arif, Trubus Rahadiansyah, Dinilai, Baru, Trubus, Ari, Lama, Pemkot, Direktur IndoStrategi Research, Analis Politik, Imam Budi Hartono</t>
+        </is>
       </c>
       <c r="B82" t="n">
         <v>0</v>
@@ -10885,8 +11047,10 @@
       </c>
     </row>
     <row r="83">
-      <c r="A83" t="n">
-        <v>0</v>
+      <c r="A83" t="inlineStr">
+        <is>
+          <t>Lilipaly, Alhasil, Persija, Yusuf, Pato, Michael Krmencik, Andritany, Diego, Riko Simanjuntak, Nur Hardianto, Krmencik, Borneo FC, Macan, Andre Luiz Alves Santos, Thomas Jens Uwe Doll</t>
+        </is>
       </c>
       <c r="B83" t="n">
         <v>0</v>
@@ -11016,8 +11180,10 @@
       </c>
     </row>
     <row r="84">
-      <c r="A84" t="n">
-        <v>0</v>
+      <c r="A84" t="inlineStr">
+        <is>
+          <t>BPBD Kulon Progo, Beras, Pelaksana, Joko Satyo Agus Nahrowi, Dukuh Kalimenur, Sen, Papah, Eko Yulianto, Kalimenur, Eko, Joko, Rupiah, Sungai Kanjangan, Banjir, Sawijan, Kapanewon, Sungai Papah</t>
+        </is>
       </c>
       <c r="B84" t="n">
         <v>0</v>
@@ -11154,8 +11320,10 @@
       </c>
     </row>
     <row r="85">
-      <c r="A85" t="n">
-        <v>0</v>
+      <c r="A85" t="inlineStr">
+        <is>
+          <t>Puskesmas, Tersangka, Pemicu Banjir Bandang, Leuwigajah, NN, Dedi, Kadiv Humas Polri Irjen Dedi Prasetyo, Pelaksana BPBD, Manggungsari, Edi, Riaz Maftuh, Polisi, Yani, Gunung Geulis, Mobil, Mapolres, Dilansir, Chang Shin Shang, Kasatlantas Polres, Atang, Dian, Anaga, Ee Huzi Abdurohman, Kombes Pol K Yani Sudarto, Atang Sutarno, Kasat Reskrim Polres, Ee Huzi, Direskrimum Polda, Palabuhanratu, Korban, China, TKP, Direktur Keselamatan Perkeretaapian Kementerian Perhubungan Edi Nursalam, Polri, Sawahdadap, Rifky, Satreskrim Polres, Campakamekar, Riaz, AKP Dian Purnomo, Imron, Rifky Wijaksana, Sindangraja, AKP Anaga Budiharso</t>
+        </is>
       </c>
       <c r="B85" t="n">
         <v>0</v>
@@ -11380,8 +11548,10 @@
       </c>
     </row>
     <row r="86">
-      <c r="A86" t="n">
-        <v>0</v>
+      <c r="A86" t="inlineStr">
+        <is>
+          <t>BMKG</t>
+        </is>
       </c>
       <c r="B86" t="n">
         <v>0</v>
@@ -11482,8 +11652,10 @@
       </c>
     </row>
     <row r="87">
-      <c r="A87" t="n">
-        <v>0</v>
+      <c r="A87" t="inlineStr">
+        <is>
+          <t>Kepala Badan Nasional Penanggulangan Bencana Suharyanto, Jokowi, Media</t>
+        </is>
       </c>
       <c r="B87" t="n">
         <v>0</v>
@@ -11594,8 +11766,10 @@
       </c>
     </row>
     <row r="88">
-      <c r="A88" t="n">
-        <v>0</v>
+      <c r="A88" t="inlineStr">
+        <is>
+          <t>Sekuriti Pantai Marina, Kompol Dicky Hermansyah, Wimbo, Pantai Marina, Wimbo Prastowo, Kapolsek, MCC, Villa Marina</t>
+        </is>
       </c>
       <c r="B88" t="n">
         <v>0</v>
@@ -11723,8 +11897,10 @@
       </c>
     </row>
     <row r="89">
-      <c r="A89" t="n">
-        <v>0</v>
+      <c r="A89" t="inlineStr">
+        <is>
+          <t>Pengungsi, Sitaro Evangelian Sasingen, Sitaro, KecamatanSiau</t>
+        </is>
       </c>
       <c r="B89" t="n">
         <v>0</v>
@@ -11833,8 +12009,10 @@
       </c>
     </row>
     <row r="90">
-      <c r="A90" t="n">
-        <v>0</v>
+      <c r="A90" t="inlineStr">
+        <is>
+          <t>Pemkab, Herman Suherman, Bupati</t>
+        </is>
       </c>
       <c r="B90" t="n">
         <v>0</v>
@@ -11950,8 +12128,10 @@
       </c>
     </row>
     <row r="91">
-      <c r="A91" t="n">
-        <v>0</v>
+      <c r="A91" t="inlineStr">
+        <is>
+          <t>Kasatlantas Polrestabes, Pasar, AKBP Ariek Indra Sentanu, Rumah Sakit, Persimpangan, Ariek</t>
+        </is>
       </c>
       <c r="B91" t="n">
         <v>0</v>
@@ -12060,8 +12240,10 @@
       </c>
     </row>
     <row r="92">
-      <c r="A92" t="n">
-        <v>0</v>
+      <c r="A92" t="inlineStr">
+        <is>
+          <t>Hendy, Damkar, Pemkab, Sungai, Sungai Jompo, Sungai Kali Jompo, Sungai Bedadung, Dilansir</t>
+        </is>
       </c>
       <c r="B92" t="n">
         <v>0</v>
@@ -12175,8 +12357,10 @@
       </c>
     </row>
     <row r="93">
-      <c r="A93" t="n">
-        <v>0</v>
+      <c r="A93" t="inlineStr">
+        <is>
+          <t>Sastrawan, I Nyoman Sastrawan, Pendem, Supervisor Teknik ULP, Ridwan Islami, Pelabuhan Gilimanuk</t>
+        </is>
       </c>
       <c r="B93" t="n">
         <v>0</v>
@@ -12291,8 +12475,10 @@
       </c>
     </row>
     <row r="94">
-      <c r="A94" t="n">
-        <v>0</v>
+      <c r="A94" t="inlineStr">
+        <is>
+          <t>Kebayoran Lama, Mampang Prapatan, Info Prakiraan Wilayah Potensi, BPBD DKI, DKI, Kebayoran Baru, Pasar, Zona Menengah</t>
+        </is>
       </c>
       <c r="B94" t="n">
         <v>0</v>
@@ -12416,8 +12602,10 @@
       </c>
     </row>
     <row r="95">
-      <c r="A95" t="n">
-        <v>0</v>
+      <c r="A95" t="inlineStr">
+        <is>
+          <t>Damkar, Pertokoan, Ngabrdurosid, Tampak, Tribun</t>
+        </is>
       </c>
       <c r="B95" t="n">
         <v>0</v>
@@ -12524,8 +12712,10 @@
       </c>
     </row>
     <row r="96">
-      <c r="A96" t="n">
-        <v>0</v>
+      <c r="A96" t="inlineStr">
+        <is>
+          <t>Diah, SMA, Prihatin, Siti, Ketua, Baznas, BPBD DKI, Prihatin Budi Santoso, Allah, Warsono, RW, Kemensos, Pendataan, Bantuan</t>
+        </is>
       </c>
       <c r="B96" t="n">
         <v>0</v>
@@ -12741,8 +12931,10 @@
       </c>
     </row>
     <row r="97">
-      <c r="A97" t="n">
-        <v>0</v>
+      <c r="A97" t="inlineStr">
+        <is>
+          <t>Adit, Kebayoran Lama, DKI, BPDB, Baru, Seskoal, JPO, Cipulir</t>
+        </is>
       </c>
       <c r="B97" t="n">
         <v>0</v>
@@ -12853,8 +13045,10 @@
       </c>
     </row>
     <row r="98">
-      <c r="A98" t="n">
-        <v>0</v>
+      <c r="A98" t="inlineStr">
+        <is>
+          <t>Pemuka Agama Protestan Pdt, Menteri Sosial Tri Rismaharini, Kemensos, Pemuka Agama Katolik Romo Agustinus Heri Wibowo, Wakil Sekretaris Komisi Fatwa MUI, Islam, Astono Chandra Dana, Pemuka Agama Hindu KRHT P, Jimmy MI Sormin, Pemuka Agama Budha Riyadi, Risma, Endang Mintarja</t>
+        </is>
       </c>
       <c r="B98" t="n">
         <v>0</v>
@@ -12902,12 +13096,12 @@
       </c>
       <c r="N98" t="inlineStr">
         <is>
-          <t>cianjur</t>
+          <t>-</t>
         </is>
       </c>
       <c r="O98" t="inlineStr">
         <is>
-          <t>jawa barat</t>
+          <t>-</t>
         </is>
       </c>
       <c r="P98" t="n">
@@ -12976,8 +13170,10 @@
       </c>
     </row>
     <row r="99">
-      <c r="A99" t="n">
-        <v>0</v>
+      <c r="A99" t="inlineStr">
+        <is>
+          <t>Sungai Woro, Nur Tjahjono Suharto, Jenarto, Aman, Kapolres, Sekretaris BPBD, Anggota, HT, Peringatan, Eko, AKBP Eko Prasetyo, Nur, Mapolres, Karangbutan, Gunung Merapi, Dam Kendalsari</t>
+        </is>
       </c>
       <c r="B99" t="n">
         <v>0</v>
@@ -13108,8 +13304,10 @@
       </c>
     </row>
     <row r="100">
-      <c r="A100" t="n">
-        <v>0</v>
+      <c r="A100" t="inlineStr">
+        <is>
+          <t>Katimbang, Kabid Drainase Dinas PU, Dinas PU, Hasna, Hidayat, Biringkanaya, Nur Hidayat, Paccerakkang, Pemkot</t>
+        </is>
       </c>
       <c r="B100" t="n">
         <v>0</v>
@@ -13235,8 +13433,10 @@
       </c>
     </row>
     <row r="101">
-      <c r="A101" t="n">
-        <v>0</v>
+      <c r="A101" t="inlineStr">
+        <is>
+          <t>Legian, Samigita, Pelaksana, Suamba, Lapangan Nyoman Suardana, Ida Bagus Surya Suamba, Pantai Legian, Arjuna, Pantauan, Tsunami Shelter, Seminyak, TJS Bianglala KSO</t>
+        </is>
       </c>
       <c r="B101" t="n">
         <v>0</v>
@@ -13369,8 +13569,10 @@
       </c>
     </row>
     <row r="102">
-      <c r="A102" t="n">
-        <v>0</v>
+      <c r="A102" t="inlineStr">
+        <is>
+          <t>DPRD, Alat Pelindung Diri, Nirwana Selle, Darna, Serikat Pekerja Nasional, Nirwana, Astaga, Pangkep, Ibunda Nirwana Selle, Mori, Kemauan Nirwana, Muhammad Safri, Tuhan, Seleb TikTok, Toraja, I Made Defri Hari Jonathan, SMK, Moh Taufik, PT GNI, Jenazah Nirwana, Aduh, Allah SWT, I Made Defri, Kak Wana, Tungku Smelter PT GNI, Made, Koordinator Eksekutif Jatam, Sidrap</t>
+        </is>
       </c>
       <c r="B102" t="n">
         <v>0</v>
@@ -13594,8 +13796,10 @@
       </c>
     </row>
     <row r="103">
-      <c r="A103" t="n">
-        <v>0</v>
+      <c r="A103" t="inlineStr">
+        <is>
+          <t>Api, Harso Wicaksono, BBM, Muklason, Kompol Muklason, Yahya, SPBU, Bobang</t>
+        </is>
       </c>
       <c r="B103" t="n">
         <v>0</v>
@@ -13706,8 +13910,10 @@
       </c>
     </row>
     <row r="104">
-      <c r="A104" t="n">
-        <v>0</v>
+      <c r="A104" t="inlineStr">
+        <is>
+          <t>Pantai Bahagia, Dani, Camat, Lukman Hakim, Pantai Bakti, Kalak BPBD, Pantai, Muaragembong, Lukman</t>
+        </is>
       </c>
       <c r="B104" t="n">
         <v>0</v>
@@ -13820,8 +14026,10 @@
       </c>
     </row>
     <row r="105">
-      <c r="A105" t="n">
-        <v>0</v>
+      <c r="A105" t="inlineStr">
+        <is>
+          <t>BPBD, Theofilo, Paledang, Bapak Bunyamin, Theofilo Patricinio Freitas</t>
+        </is>
       </c>
       <c r="B105" t="n">
         <v>0</v>
@@ -13934,8 +14142,10 @@
       </c>
     </row>
     <row r="106">
-      <c r="A106" t="n">
-        <v>0</v>
+      <c r="A106" t="inlineStr">
+        <is>
+          <t>BPDB Polwewali Mandar, Andi Affandi, Affandi, Hujan, Andi Affandi Rahman</t>
+        </is>
       </c>
       <c r="B106" t="n">
         <v>0</v>
@@ -14051,8 +14261,10 @@
       </c>
     </row>
     <row r="107">
-      <c r="A107" t="n">
-        <v>0</v>
+      <c r="A107" t="inlineStr">
+        <is>
+          <t>Angkatan Kidul, Karangwono, Mirza Nur Hidayat, Sinomwidodo, Mirza, Korban, Suami, Angkatan Lor</t>
+        </is>
       </c>
       <c r="B107" t="n">
         <v>0</v>
@@ -14166,8 +14378,10 @@
       </c>
     </row>
     <row r="108">
-      <c r="A108" t="n">
-        <v>0</v>
+      <c r="A108" t="inlineStr">
+        <is>
+          <t>Sanindo, Rijaya, Koordinator Satuan Pelayanan, AWS, Nataru, Tigaras, Ambarita, Sumatera, BMKG</t>
+        </is>
       </c>
       <c r="B108" t="n">
         <v>0</v>
@@ -14279,8 +14493,10 @@
       </c>
     </row>
     <row r="109">
-      <c r="A109" t="n">
-        <v>0</v>
+      <c r="A109" t="inlineStr">
+        <is>
+          <t>Moel, Moel Wahyono, Petugas, Kapten Dantim SAR, DVI Polri</t>
+        </is>
       </c>
       <c r="B109" t="n">
         <v>0</v>
@@ -14393,8 +14609,10 @@
       </c>
     </row>
     <row r="110">
-      <c r="A110" t="n">
-        <v>0</v>
+      <c r="A110" t="inlineStr">
+        <is>
+          <t>Banjir, Sutarno</t>
+        </is>
       </c>
       <c r="B110" t="n">
         <v>0</v>
@@ -14516,8 +14734,10 @@
       </c>
     </row>
     <row r="111">
-      <c r="A111" t="n">
-        <v>0</v>
+      <c r="A111" t="inlineStr">
+        <is>
+          <t>Arseven, Bupati, Tuhan, Pemkab, HS, AR Seven, Sarongge, Palangon, Pak Hasan, Arseven Coffe Corner, Ar Seven, MI, SD Khoiru Ummah, Warung Sate Shinta</t>
+        </is>
       </c>
       <c r="B111" t="n">
         <v>0</v>
@@ -14692,8 +14912,10 @@
       </c>
     </row>
     <row r="112">
-      <c r="A112" t="n">
-        <v>0</v>
+      <c r="A112" t="inlineStr">
+        <is>
+          <t>DPT, Cilebut, Perbaikan, Jl, Ali, Subbidang Tata Usaha UPT Perbaikan, Entus Supriatna, Entus</t>
+        </is>
       </c>
       <c r="B112" t="n">
         <v>0</v>
@@ -14812,8 +15034,10 @@
       </c>
     </row>
     <row r="113">
-      <c r="A113" t="n">
-        <v>0</v>
+      <c r="A113" t="inlineStr">
+        <is>
+          <t>Agus Hanif, Rumahnya, Pandansari, Gelombang, Jembatan Bedono, Aisyah, Dukuh Pandansari, Bedono, Dukuh Pandasari, Agus</t>
+        </is>
       </c>
       <c r="B113" t="n">
         <v>0</v>
@@ -14943,8 +15167,10 @@
       </c>
     </row>
     <row r="114">
-      <c r="A114" t="n">
-        <v>0</v>
+      <c r="A114" t="inlineStr">
+        <is>
+          <t>M Faridzal Gumay, Jabodetabek, BPBD Tangsel, BRIN Erma Yulihastin, Gumay, Erma, SOP BPBD, BMKG</t>
+        </is>
       </c>
       <c r="B114" t="n">
         <v>0</v>
@@ -15080,8 +15306,10 @@
       </c>
     </row>
     <row r="115">
-      <c r="A115" t="n">
-        <v>0</v>
+      <c r="A115" t="inlineStr">
+        <is>
+          <t>Rangkap Lalu Jaenun, Syahnan, KEK Mandalika, Ridwan, Mertak, PT, Banjir, Kepala, Sirkuit Mandalika</t>
+        </is>
       </c>
       <c r="B115" t="n">
         <v>0</v>
@@ -15207,8 +15435,10 @@
       </c>
     </row>
     <row r="116">
-      <c r="A116" t="n">
-        <v>0</v>
+      <c r="A116" t="inlineStr">
+        <is>
+          <t>TN Baluran, Savana Bekol, Arif, Bekol, Baluran</t>
+        </is>
       </c>
       <c r="B116" t="n">
         <v>0</v>
@@ -15320,8 +15550,10 @@
       </c>
     </row>
     <row r="117">
-      <c r="A117" t="n">
-        <v>0</v>
+      <c r="A117" t="inlineStr">
+        <is>
+          <t>Cidawolong, Karangligar, Yasin Nasrudin, Kulon, Tanjungmekar, Yasin</t>
+        </is>
       </c>
       <c r="B117" t="n">
         <v>0</v>
@@ -15438,8 +15670,10 @@
       </c>
     </row>
     <row r="118">
-      <c r="A118" t="n">
-        <v>0</v>
+      <c r="A118" t="inlineStr">
+        <is>
+          <t>Pasar, Mapolsek, Pihaknya, Syamsuri, Kapolsek, Iptu Muhammad Syamsuri, Banjir</t>
+        </is>
       </c>
       <c r="B118" t="n">
         <v>0</v>
@@ -15553,8 +15787,10 @@
       </c>
     </row>
     <row r="119">
-      <c r="A119" t="n">
-        <v>0</v>
+      <c r="A119" t="inlineStr">
+        <is>
+          <t>SMK Pertanian, Nia, Bupati, Herman, Pasirsembung, Pemkab, Pantauan, Sirnagalih, TPAS, TPAS Pasirsembung, Cipendawa, Herman Suherman, BMKG</t>
+        </is>
       </c>
       <c r="B119" t="n">
         <v>0</v>
@@ -15698,8 +15934,10 @@
       </c>
     </row>
     <row r="120">
-      <c r="A120" t="n">
-        <v>0</v>
+      <c r="A120" t="inlineStr">
+        <is>
+          <t>BPBD, Suwardi, Kepala BMKG, Kulon</t>
+        </is>
       </c>
       <c r="B120" t="n">
         <v>0</v>
@@ -15828,8 +16066,10 @@
       </c>
     </row>
     <row r="121">
-      <c r="A121" t="n">
-        <v>0</v>
+      <c r="A121" t="inlineStr">
+        <is>
+          <t>MH Thamrin, Nataru, Polda, Operasi Lilin, Summarecon, Pos Bloc, GBK, Bundaran HI, Panggung Hiburan Dijaga, Ragunan, MRT Bundaran HI, Ancol, Zulpan, BSD, PIK, Sarinah, Siaga Polda, Aquarium, Patung, TMII, Blok M, Senopati, Tua</t>
+        </is>
       </c>
       <c r="B121" t="n">
         <v>0</v>
@@ -15877,12 +16117,12 @@
       </c>
       <c r="N121" t="inlineStr">
         <is>
-          <t>tangerang</t>
+          <t>jakarta timur</t>
         </is>
       </c>
       <c r="O121" t="inlineStr">
         <is>
-          <t>banten</t>
+          <t>dki jakarta</t>
         </is>
       </c>
       <c r="P121" t="n">
@@ -15968,8 +16208,10 @@
       </c>
     </row>
     <row r="122">
-      <c r="A122" t="n">
-        <v>0</v>
+      <c r="A122" t="inlineStr">
+        <is>
+          <t>Medaeng, Bungurasih, Kades Bunggurasih Eko Julianto, PLN</t>
+        </is>
       </c>
       <c r="B122" t="n">
         <v>0</v>
@@ -16084,8 +16326,10 @@
       </c>
     </row>
     <row r="123">
-      <c r="A123" t="n">
-        <v>0</v>
+      <c r="A123" t="inlineStr">
+        <is>
+          <t>Kawasan Cileueur River Walk, Prasarana Permukiman Wilayah, Fery Yuliatna, Pedestrian, Fery, Serah, DPRKPLH, PPK Pengembangan Kawasan Permukiman, Feri, Ipal, Cileueur River Walk</t>
+        </is>
       </c>
       <c r="B123" t="n">
         <v>0</v>
@@ -16217,8 +16461,10 @@
       </c>
     </row>
     <row r="124">
-      <c r="A124" t="n">
-        <v>0</v>
+      <c r="A124" t="inlineStr">
+        <is>
+          <t>Yusuf, RSUD Palabuhanratu, Plt Dirut RSUD Palabuhanratu, Yusuf Eriadi, IGD, Luhung Budiailmiawan</t>
+        </is>
       </c>
       <c r="B124" t="n">
         <v>0</v>
@@ -16266,12 +16512,12 @@
       </c>
       <c r="N124" t="inlineStr">
         <is>
-          <t>sukabumi</t>
+          <t>-</t>
         </is>
       </c>
       <c r="O124" t="inlineStr">
         <is>
-          <t>jawa barat</t>
+          <t>-</t>
         </is>
       </c>
       <c r="P124" t="n">
@@ -16336,8 +16582,10 @@
       </c>
     </row>
     <row r="125">
-      <c r="A125" t="n">
-        <v>0</v>
+      <c r="A125" t="inlineStr">
+        <is>
+          <t>Manajer Riset MSI Adi Imam Taufik, PKL, Wakil Wali, Pemkot, Tangsel, Adi, Survei, Benyamin, Wali, Pilar, MSI</t>
+        </is>
       </c>
       <c r="B125" t="n">
         <v>0</v>
@@ -16478,8 +16726,10 @@
       </c>
     </row>
     <row r="126">
-      <c r="A126" t="n">
-        <v>0</v>
+      <c r="A126" t="inlineStr">
+        <is>
+          <t>Toraja, Lurah Pusserren, Asman, Harton</t>
+        </is>
       </c>
       <c r="B126" t="n">
         <v>0</v>
@@ -16608,8 +16858,10 @@
       </c>
     </row>
     <row r="127">
-      <c r="A127" t="n">
-        <v>0</v>
+      <c r="A127" t="inlineStr">
+        <is>
+          <t>Matua, Yani Hartono, BPBD, Kerusakan, Yani, Mumbu, Sekretaris Badan Penanggulangan Bencana Daerah, BMKG</t>
+        </is>
       </c>
       <c r="B127" t="n">
         <v>0</v>
@@ -16725,8 +16977,10 @@
       </c>
     </row>
     <row r="128">
-      <c r="A128" t="n">
-        <v>0</v>
+      <c r="A128" t="inlineStr">
+        <is>
+          <t>Krokosono Panggung Lor, Kapolsek, Kompol Budi Abadi, Sungai, Yesus Tanah Mas, Polisi, Erian Dita, Relawan, Katolik Hati, Mayat, Kanal</t>
+        </is>
       </c>
       <c r="B128" t="n">
         <v>0</v>
@@ -16832,8 +17086,10 @@
       </c>
     </row>
     <row r="129">
-      <c r="A129" t="n">
-        <v>0</v>
+      <c r="A129" t="inlineStr">
+        <is>
+          <t>BPBD, Pelaksana, Martinus Budi Prasetya, Ketitang Wetan, Anton, Sungai Kaliombo, Banjir</t>
+        </is>
       </c>
       <c r="B129" t="n">
         <v>0</v>
@@ -16942,8 +17198,10 @@
       </c>
     </row>
     <row r="130">
-      <c r="A130" t="n">
-        <v>0</v>
+      <c r="A130" t="inlineStr">
+        <is>
+          <t>Reni, PKS, Reni Astuti, SDM, Wakil DPRD, Sekda, Pak Ikhsan</t>
+        </is>
       </c>
       <c r="B130" t="n">
         <v>0</v>
@@ -17067,8 +17325,10 @@
       </c>
     </row>
     <row r="131">
-      <c r="A131" t="n">
-        <v>0</v>
+      <c r="A131" t="inlineStr">
+        <is>
+          <t>Heru Budi Hartono, Heru Budi, Heru, Hari, Wali, DKI, Dinas Bina, M Anwar, Afan Adriansyah, Asisten Pembangunan, Gubernur DKI, Kepala Dinas Bina, Hari Nugroho</t>
+        </is>
       </c>
       <c r="B131" t="n">
         <v>0</v>
@@ -17201,8 +17461,10 @@
       </c>
     </row>
     <row r="132">
-      <c r="A132" t="n">
-        <v>0</v>
+      <c r="A132" t="inlineStr">
+        <is>
+          <t>Distrik, Polisi, Kabid Humas Polda, Deiyai, Kombes Ahmad Musthofa, Dilansir</t>
+        </is>
       </c>
       <c r="B132" t="n">
         <v>0</v>
@@ -17310,8 +17572,10 @@
       </c>
     </row>
     <row r="133">
-      <c r="A133" t="n">
-        <v>0</v>
+      <c r="A133" t="inlineStr">
+        <is>
+          <t>Operator, Poros, Kasat Lantas Polres, Fadli, AKP Supriyanto, Tim SAR, Supriyanto</t>
+        </is>
       </c>
       <c r="B133" t="n">
         <v>0</v>
@@ -17433,8 +17697,10 @@
       </c>
     </row>
     <row r="134">
-      <c r="A134" t="n">
-        <v>0</v>
+      <c r="A134" t="inlineStr">
+        <is>
+          <t>Polsek, Kebetulan, Dindin Sukaya, TNI, Dindin</t>
+        </is>
       </c>
       <c r="B134" t="n">
         <v>0</v>
@@ -17553,8 +17819,10 @@
       </c>
     </row>
     <row r="135">
-      <c r="A135" t="n">
-        <v>0</v>
+      <c r="A135" t="inlineStr">
+        <is>
+          <t>Serdang Bedagai, Amenson, BKSDA Sumatera, Rian, Amenson Girsang, Pemilik, Seksi Perencanaan</t>
+        </is>
       </c>
       <c r="B135" t="n">
         <v>0</v>
@@ -17674,8 +17942,10 @@
       </c>
     </row>
     <row r="136">
-      <c r="A136" t="n">
-        <v>0</v>
+      <c r="A136" t="inlineStr">
+        <is>
+          <t>IPU, Pantai Marina, Mbak Ita, Ita, Banjir, Villa Marina</t>
+        </is>
       </c>
       <c r="B136" t="n">
         <v>0</v>
@@ -17793,8 +18063,10 @@
       </c>
     </row>
     <row r="137">
-      <c r="A137" t="n">
-        <v>0</v>
+      <c r="A137" t="inlineStr">
+        <is>
+          <t>Andaru, Purwokerto, Andaru Budilaksono</t>
+        </is>
       </c>
       <c r="B137" t="n">
         <v>0</v>
@@ -17902,8 +18174,10 @@
       </c>
     </row>
     <row r="138">
-      <c r="A138" t="n">
-        <v>0</v>
+      <c r="A138" t="inlineStr">
+        <is>
+          <t>Adit, Sardi, Api, Penyelamatan, TV, Kebon Jeruk</t>
+        </is>
       </c>
       <c r="B138" t="n">
         <v>0</v>
@@ -18016,8 +18290,10 @@
       </c>
     </row>
     <row r="139">
-      <c r="A139" t="n">
-        <v>0</v>
+      <c r="A139" t="inlineStr">
+        <is>
+          <t>Opu, Gelar Opu, Perintis Pergerakan Kebangsaan Kemerdekaan, Opu Daeng Mawellu, Mudehang, Islam, Partai Awalnya Opu Daeng Risadju, Ayahnya, Raja, Belanda, Akhir Hayat Opu Daeng Risadju Opu Daeng Risadju, PSII, Mengenyam Pendidikan Formal, Lontara, Haji Muhammad Daud, Indonesia, Perang, Dosen Ilmu Sejarah, Lokkoe, Famajjah, Fakultas Ilmu Budaya Universitas Hasanuddin, Bugis, Dewan Adat, Muhammad Abdullah To Bareseng, Arab, Risadju, TNI, Opu Daeng Risadju, Suriadi, Dr Suriadi Mappangara M Hum, Republik Indonesia</t>
+        </is>
       </c>
       <c r="B139" t="n">
         <v>0</v>
@@ -18250,8 +18526,10 @@
       </c>
     </row>
     <row r="140">
-      <c r="A140" t="n">
-        <v>0</v>
+      <c r="A140" t="inlineStr">
+        <is>
+          <t>Panakukkang, Tombolopao, Somba Upu, Pangkep, Biringkanaya, Baru, Mangarabombang, Polombangkeng, Tondong Tallasa, Pattalasang, BMKG, Moncong Loe</t>
+        </is>
       </c>
       <c r="B140" t="n">
         <v>0</v>
@@ -18364,8 +18642,10 @@
       </c>
     </row>
     <row r="141">
-      <c r="A141" t="n">
-        <v>0</v>
+      <c r="A141" t="inlineStr">
+        <is>
+          <t>BPBD, Husni Thamrin, Husni, SK Wali, Tim Reaksi Cepat, BMKG</t>
+        </is>
       </c>
       <c r="B141" t="n">
         <v>0</v>
@@ -18477,8 +18757,10 @@
       </c>
     </row>
     <row r="142">
-      <c r="A142" t="n">
-        <v>0</v>
+      <c r="A142" t="inlineStr">
+        <is>
+          <t>Tim Satgas TNI AL Peduli, Letkol Mar Edo Sidharta Halilintar M, Kompol, Fauzi Noviandi, Rifki Mauladi Saiful Bahri, M Ikhsan Sp F, Cibulakan, Kontributor, Biddokes Polda, RSUD Sayang, RSUD, Tim DVI Polda, RSUD Cimacan, Ikhsan</t>
+        </is>
       </c>
       <c r="B142" t="n">
         <v>0</v>
@@ -18618,8 +18900,10 @@
       </c>
     </row>
     <row r="143">
-      <c r="A143" t="n">
-        <v>0</v>
+      <c r="A143" t="inlineStr">
+        <is>
+          <t>Gunungkidul, BMKG</t>
+        </is>
       </c>
       <c r="B143" t="n">
         <v>0</v>
@@ -18720,8 +19004,10 @@
       </c>
     </row>
     <row r="144">
-      <c r="A144" t="n">
-        <v>0</v>
+      <c r="A144" t="inlineStr">
+        <is>
+          <t>Saan, Doli, JR, Hasyim, UU, Ketua KPU, Pemilu, KPU, DPR, MK, UU Pemilu, Sekretaris Fraksi NasDem DPR</t>
+        </is>
       </c>
       <c r="B144" t="n">
         <v>0</v>
@@ -18885,8 +19171,10 @@
       </c>
     </row>
     <row r="145">
-      <c r="A145" t="n">
-        <v>0</v>
+      <c r="A145" t="inlineStr">
+        <is>
+          <t>Gunungpuyuh, BPBD, Jenderal Sudirman, Pelaksana BPBD, Imran, Rumah Tesa, Zul, Badan Penanggulangan Bencana Daerah, Zulkarnain, Imran Wardhani, SKPD, Zulkarnain Barhami, Kesiapsiagaan BPBD</t>
+        </is>
       </c>
       <c r="B145" t="n">
         <v>0</v>
@@ -19040,8 +19328,10 @@
       </c>
     </row>
     <row r="146">
-      <c r="A146" t="n">
-        <v>0</v>
+      <c r="A146" t="inlineStr">
+        <is>
+          <t>BPBD, Pelaksana BPBD, Pemkab, Pacar, Karangjompo, Budi Rahardjo, Fadia Arafiq, Samborejo, Budi</t>
+        </is>
       </c>
       <c r="B146" t="n">
         <v>0</v>
@@ -19166,8 +19456,10 @@
       </c>
     </row>
     <row r="147">
-      <c r="A147" t="n">
-        <v>0</v>
+      <c r="A147" t="inlineStr">
+        <is>
+          <t>BMKG, Gempa</t>
+        </is>
       </c>
       <c r="B147" t="n">
         <v>0</v>
@@ -19268,8 +19560,10 @@
       </c>
     </row>
     <row r="148">
-      <c r="A148" t="n">
-        <v>0</v>
+      <c r="A148" t="inlineStr">
+        <is>
+          <t>Eka Tirtana, I Putu Eka Putra Tirtana, Logistik BPBD, PLN</t>
+        </is>
       </c>
       <c r="B148" t="n">
         <v>0</v>
@@ -19386,8 +19680,10 @@
       </c>
     </row>
     <row r="149">
-      <c r="A149" t="n">
-        <v>0</v>
+      <c r="A149" t="inlineStr">
+        <is>
+          <t>BMKG, Gempa</t>
+        </is>
       </c>
       <c r="B149" t="n">
         <v>0</v>
@@ -19494,8 +19790,10 @@
       </c>
     </row>
     <row r="150">
-      <c r="A150" t="n">
-        <v>0</v>
+      <c r="A150" t="inlineStr">
+        <is>
+          <t>PKL, Kapolres, Aszhari, Polisi, Pemkab, Perdagangan, Iwan Ridwan, Puslabfor Mabes Polri, AKBP Aszhari Kurniawan, Iwan</t>
+        </is>
       </c>
       <c r="B150" t="n">
         <v>0</v>
@@ -19616,8 +19914,10 @@
       </c>
     </row>
     <row r="151">
-      <c r="A151" t="n">
-        <v>0</v>
+      <c r="A151" t="inlineStr">
+        <is>
+          <t>Atang, Nugi Nogroho, Kawasan Gunung Geulis, Pelaksana BPBD, Atang Sutarno, Gunung Geulis, Sawahdadap, Nugi</t>
+        </is>
       </c>
       <c r="B151" t="n">
         <v>0</v>
@@ -19749,8 +20049,10 @@
       </c>
     </row>
     <row r="152">
-      <c r="A152" t="n">
-        <v>0</v>
+      <c r="A152" t="inlineStr">
+        <is>
+          <t>Pangkep, Irwan, Irwan Slamet, Ellie</t>
+        </is>
       </c>
       <c r="B152" t="n">
         <v>0</v>
@@ -19902,8 +20204,10 @@
       </c>
     </row>
     <row r="153">
-      <c r="A153" t="n">
-        <v>0</v>
+      <c r="A153" t="inlineStr">
+        <is>
+          <t>Iptu Mohammad Budi Santoso, Keramaian, Prakiraan Kondisi Gelombang Wilayah Perairan, Masalembo, Budi</t>
+        </is>
       </c>
       <c r="B153" t="n">
         <v>0</v>
@@ -20020,8 +20324,10 @@
       </c>
     </row>
     <row r="154">
-      <c r="A154" t="n">
-        <v>0</v>
+      <c r="A154" t="inlineStr">
+        <is>
+          <t>TPK, Jhony Tamailang, Minut, Kasat Lantas Polres Minut Iptu Julio J Tampoi, Julio</t>
+        </is>
       </c>
       <c r="B154" t="n">
         <v>0</v>
@@ -20132,8 +20438,10 @@
       </c>
     </row>
     <row r="155">
-      <c r="A155" t="n">
-        <v>0</v>
+      <c r="A155" t="inlineStr">
+        <is>
+          <t>Termulus, C Penanggungan, Pantura, Kelurahah, Stasiun Besar, Sukareja, Muktiharjo Lor, Kulon, Dukuh, Wonowoso, Kebonadem, Musala Bani Ilyas, Cangkring, Plamongan, Kalisari, Putatsari, BNPB, Setrokalangan</t>
+        </is>
       </c>
       <c r="B155" t="n">
         <v>0</v>
@@ -20305,8 +20613,10 @@
       </c>
     </row>
     <row r="156">
-      <c r="A156" t="n">
-        <v>0</v>
+      <c r="A156" t="inlineStr">
+        <is>
+          <t>Tanah Baru, BPBD, Jabodetabek, Erna Yulihastin, Halang, Cibulu, BRIN, Theo, Erma, Theofilo Patricinio Freitas</t>
+        </is>
       </c>
       <c r="B156" t="n">
         <v>0</v>
@@ -20433,8 +20743,10 @@
       </c>
     </row>
     <row r="157">
-      <c r="A157" t="n">
-        <v>0</v>
+      <c r="A157" t="inlineStr">
+        <is>
+          <t>Caracas, Khawatir, Mh Khadafi Mufti, Khadafi, Kepala UPT Damkar Satpol PP</t>
+        </is>
       </c>
       <c r="B157" t="n">
         <v>0</v>
@@ -20555,8 +20867,10 @@
       </c>
     </row>
     <row r="158">
-      <c r="A158" t="n">
-        <v>0</v>
+      <c r="A158" t="inlineStr">
+        <is>
+          <t>Danau Sidenreng, Sidrap, Basri</t>
+        </is>
       </c>
       <c r="B158" t="n">
         <v>0</v>
@@ -20673,8 +20987,10 @@
       </c>
     </row>
     <row r="159">
-      <c r="A159" t="n">
-        <v>0</v>
+      <c r="A159" t="inlineStr">
+        <is>
+          <t>Kepala BPBD Tana Toraja Christian Batara Sakkung, Dinas Sosial, Miallo, Dinsos, Sembako, Iptu Andarias Tonapa, Kapolsek, Turbinnya, Mangose</t>
+        </is>
       </c>
       <c r="B159" t="n">
         <v>0</v>
@@ -20793,8 +21109,10 @@
       </c>
     </row>
     <row r="160">
-      <c r="A160" t="n">
-        <v>0</v>
+      <c r="A160" t="inlineStr">
+        <is>
+          <t>Astam, Korban Astam, Palmyra, Pemilik, Kadek</t>
+        </is>
       </c>
       <c r="B160" t="n">
         <v>0</v>
@@ -20913,8 +21231,10 @@
       </c>
     </row>
     <row r="161">
-      <c r="A161" t="n">
-        <v>0</v>
+      <c r="A161" t="inlineStr">
+        <is>
+          <t>SAR, Tim SAR Gabungan, Jebrod, Jumaril, Cijedil, Kepala Kantor SAR</t>
+        </is>
       </c>
       <c r="B161" t="n">
         <v>0</v>
@@ -20962,7 +21282,7 @@
       </c>
       <c r="N161" t="inlineStr">
         <is>
-          <t>bandung</t>
+          <t>cianjur</t>
         </is>
       </c>
       <c r="O161" t="inlineStr">
@@ -21036,8 +21356,10 @@
       </c>
     </row>
     <row r="162">
-      <c r="A162" t="n">
-        <v>0</v>
+      <c r="A162" t="inlineStr">
+        <is>
+          <t>Bosnia Sarajevo, Institut, Reuters, Sungai Nervion, Prancis Joana Host, Czech Television, Meteo France, Celcius, Leon, Robert Vautard, Polandia, Hungaria, Cantabria, Copernicus Climate Change Service Uni Eropa, Freja Vamborg, Jerman, Laplace Prancis, Jahorina, Matahari, Bilbao, Klimatologi Swiss, Tahun Baru, Pakistan, Asturias, Imperial College London, Dr Friederike Otto</t>
+        </is>
       </c>
       <c r="B162" t="n">
         <v>0</v>
@@ -21188,8 +21510,10 @@
       </c>
     </row>
     <row r="163">
-      <c r="A163" t="n">
-        <v>0</v>
+      <c r="A163" t="inlineStr">
+        <is>
+          <t>Ipda Defri, Kapolsek, Yonahes Mase, Anis, Kepala, Heri, Anis Mase</t>
+        </is>
       </c>
       <c r="B163" t="n">
         <v>0</v>
@@ -21309,8 +21633,10 @@
       </c>
     </row>
     <row r="164">
-      <c r="A164" t="n">
-        <v>0</v>
+      <c r="A164" t="inlineStr">
+        <is>
+          <t>Nelayan, Sri Wahyuni, Lorok, Emas, Banjir</t>
+        </is>
       </c>
       <c r="B164" t="n">
         <v>0</v>
@@ -21425,8 +21751,10 @@
       </c>
     </row>
     <row r="165">
-      <c r="A165" t="n">
-        <v>0</v>
+      <c r="A165" t="inlineStr">
+        <is>
+          <t>Agus, Ridwan, Kemarin, Sodikin, Agus Susanto, Kepala, Wetan</t>
+        </is>
       </c>
       <c r="B165" t="n">
         <v>0</v>
@@ -21548,8 +21876,10 @@
       </c>
     </row>
     <row r="166">
-      <c r="A166" t="n">
-        <v>0</v>
+      <c r="A166" t="inlineStr">
+        <is>
+          <t>Gatot, Jaktim Gatot Sulaeman</t>
+        </is>
       </c>
       <c r="B166" t="n">
         <v>0</v>
@@ -21670,8 +22000,10 @@
       </c>
     </row>
     <row r="167">
-      <c r="A167" t="n">
-        <v>0</v>
+      <c r="A167" t="inlineStr">
+        <is>
+          <t>Dinas Lingkungan Hidup, Pomanto, Danny, Pemkot</t>
+        </is>
       </c>
       <c r="B167" t="n">
         <v>0</v>
@@ -21782,8 +22114,10 @@
       </c>
     </row>
     <row r="168">
-      <c r="A168" t="n">
-        <v>0</v>
+      <c r="A168" t="inlineStr">
+        <is>
+          <t>BMKG, Bujur, Getaran, Gempa</t>
+        </is>
       </c>
       <c r="B168" t="n">
         <v>0</v>
@@ -21894,8 +22228,10 @@
       </c>
     </row>
     <row r="169">
-      <c r="A169" t="n">
-        <v>0</v>
+      <c r="A169" t="inlineStr">
+        <is>
+          <t>RS Aisyah, Erik, AKP Gunadi, Christime Yhuwanita Anggraen, Ahmad, Kapolsek, Ratna</t>
+        </is>
       </c>
       <c r="B169" t="n">
         <v>0</v>
@@ -22011,8 +22347,10 @@
       </c>
     </row>
     <row r="170">
-      <c r="A170" t="n">
-        <v>0</v>
+      <c r="A170" t="inlineStr">
+        <is>
+          <t>Dwikorita, Malut, Indonesia, NTT, BMKG, Kepala BMKG Dwikorita, NTB</t>
+        </is>
       </c>
       <c r="B170" t="n">
         <v>0</v>
@@ -22128,8 +22466,10 @@
       </c>
     </row>
     <row r="171">
-      <c r="A171" t="n">
-        <v>0</v>
+      <c r="A171" t="inlineStr">
+        <is>
+          <t>Suramadu, Pahlawan, North Quay, Tahun, BMX, Romansa, Perumahan Citraland, Disc Jockey, Bungkul, Jembatan Suroboyo, Ngumpul, Surya Nusantara, Kawasan Grahadi Kawasan Grahadi, Apsari, Contong</t>
+        </is>
       </c>
       <c r="B171" t="n">
         <v>0</v>
@@ -22302,8 +22642,10 @@
       </c>
     </row>
     <row r="172">
-      <c r="A172" t="n">
-        <v>0</v>
+      <c r="A172" t="inlineStr">
+        <is>
+          <t>BPBD, Satriyo, Gempa Bumi, Rekonstruksi BPBD, Satriyo Nurseno</t>
+        </is>
       </c>
       <c r="B172" t="n">
         <v>0</v>
@@ -22471,8 +22813,10 @@
       </c>
     </row>
     <row r="173">
-      <c r="A173" t="n">
-        <v>0</v>
+      <c r="A173" t="inlineStr">
+        <is>
+          <t>Perbekel, Pasca, Komang Guna, Pleton Fire Inspektur, I Nyoman Suarjana</t>
+        </is>
       </c>
       <c r="B173" t="n">
         <v>0</v>
@@ -22577,8 +22921,10 @@
       </c>
     </row>
     <row r="174">
-      <c r="A174" t="n">
-        <v>0</v>
+      <c r="A174" t="inlineStr">
+        <is>
+          <t>Syamtalira Aron, Camat Syamtalira Aron, Kausar</t>
+        </is>
       </c>
       <c r="B174" t="n">
         <v>0</v>
@@ -22687,8 +23033,10 @@
       </c>
     </row>
     <row r="175">
-      <c r="A175" t="n">
-        <v>0</v>
+      <c r="A175" t="inlineStr">
+        <is>
+          <t>BPBD, Petukangan, Michael Sitanggang, Michael, Damkar, BPBD DKI, DKI, Dinas Bina, Dinas SDA, Bina, Dinas Gulkarmat, Cipulir</t>
+        </is>
       </c>
       <c r="B175" t="n">
         <v>0</v>
@@ -22811,8 +23159,10 @@
       </c>
     </row>
     <row r="176">
-      <c r="A176" t="n">
-        <v>0</v>
+      <c r="A176" t="inlineStr">
+        <is>
+          <t>SMA, Youtube, Pihak TPS, Muchamad Ikhsan, Pandawara, Ridwan Kamil, Indonesia, TPS, Instagram, Agung Permana, Gilang Rahma, TikTok, Ikhsan, Kiprah Pandawara, Aksi Pandawara, Wetan, Rafly Pasya</t>
+        </is>
       </c>
       <c r="B176" t="n">
         <v>0</v>
@@ -22982,8 +23332,10 @@
       </c>
     </row>
     <row r="177">
-      <c r="A177" t="n">
-        <v>0</v>
+      <c r="A177" t="inlineStr">
+        <is>
+          <t>Camat, Biringkanaya, Pomanto, Danny</t>
+        </is>
       </c>
       <c r="B177" t="n">
         <v>0</v>
@@ -23097,8 +23449,10 @@
       </c>
     </row>
     <row r="178">
-      <c r="A178" t="n">
-        <v>0</v>
+      <c r="A178" t="inlineStr">
+        <is>
+          <t>Agus Yulianto, Gadudero, Risma, Agus, Rombongan Risma</t>
+        </is>
       </c>
       <c r="B178" t="n">
         <v>0</v>
@@ -23215,8 +23569,10 @@
       </c>
     </row>
     <row r="179">
-      <c r="A179" t="n">
-        <v>0</v>
+      <c r="A179" t="inlineStr">
+        <is>
+          <t>BPBD, Brawijaya, Sekretaris BPBD, Basuki Rahmat, Sobo, Mujito, Adi Sucipto, Kapten Piere Tendean, Kepiting, Ahmad Yani, Panderejo</t>
+        </is>
       </c>
       <c r="B179" t="n">
         <v>0</v>
@@ -23329,8 +23685,10 @@
       </c>
     </row>
     <row r="180">
-      <c r="A180" t="n">
-        <v>0</v>
+      <c r="A180" t="inlineStr">
+        <is>
+          <t>Riawa, Pemkab, Riase, Pelaksana BPBD Sidrap, Sudarmin, Sidrap</t>
+        </is>
       </c>
       <c r="B180" t="n">
         <v>0</v>
@@ -23446,8 +23804,10 @@
       </c>
     </row>
     <row r="181">
-      <c r="A181" t="n">
-        <v>0</v>
+      <c r="A181" t="inlineStr">
+        <is>
+          <t>Ayu Dwi, Kulon Progo, Aris Widyatmoko, Ayu, Banjir, Pantai, Koordinator Lapangan Wisata Laguna, Laguna, Koordinator Satlinmas Rescue Istimewa Wilayah V Kulon Progo, Kapanewon</t>
+        </is>
       </c>
       <c r="B181" t="n">
         <v>0</v>
@@ -23571,8 +23931,10 @@
       </c>
     </row>
     <row r="182">
-      <c r="A182" t="n">
-        <v>0</v>
+      <c r="A182" t="inlineStr">
+        <is>
+          <t>Jasa Raharja, BBM, L, Bapak Presiden, Menteri Perhubungan Budi Karya Sumadi, Budi</t>
+        </is>
       </c>
       <c r="B182" t="n">
         <v>0</v>
@@ -23695,8 +24057,10 @@
       </c>
     </row>
     <row r="183">
-      <c r="A183" t="n">
-        <v>0</v>
+      <c r="A183" t="inlineStr">
+        <is>
+          <t>Wawonduru, Tajudin Hir, Sahrul, Ginte, Manggemaci</t>
+        </is>
       </c>
       <c r="B183" t="n">
         <v>0</v>
@@ -23816,8 +24180,10 @@
       </c>
     </row>
     <row r="184">
-      <c r="A184" t="n">
-        <v>0</v>
+      <c r="A184" t="inlineStr">
+        <is>
+          <t>Heru Budi Hartono, Buncit, Heru, BPBD DKI, Publik, DKI, Pramuka, Pemprov DKI, Heru Budi, Riwaty, WFO, Gubernur DKI, WFH</t>
+        </is>
       </c>
       <c r="B184" t="n">
         <v>0</v>
@@ -23955,8 +24321,10 @@
       </c>
     </row>
     <row r="185">
-      <c r="A185" t="n">
-        <v>0</v>
+      <c r="A185" t="inlineStr">
+        <is>
+          <t>Mangkang, Bhabinkamtibmas, Mangkang Wetan, Wicaksono, Instagram, Mangkang Kulon, Adi, Nomor Prasetyo, Bripka Adi Sudarmanto, Mangunharjo, Banjir, Polrestabes</t>
+        </is>
       </c>
       <c r="B185" t="n">
         <v>0</v>
@@ -24069,8 +24437,10 @@
       </c>
     </row>
     <row r="186">
-      <c r="A186" t="n">
-        <v>0</v>
+      <c r="A186" t="inlineStr">
+        <is>
+          <t>Lapak, Kebon Jeruk, Syarifudin, Petugas</t>
+        </is>
       </c>
       <c r="B186" t="n">
         <v>0</v>
@@ -24177,8 +24547,10 @@
       </c>
     </row>
     <row r="187">
-      <c r="A187" t="n">
-        <v>0</v>
+      <c r="A187" t="inlineStr">
+        <is>
+          <t>Stasiun, KA Sembrani, Solo, Pasar, Stasiun Ngrombo, Pantauan Tribun</t>
+        </is>
       </c>
       <c r="B187" t="n">
         <v>0</v>
@@ -24295,8 +24667,10 @@
       </c>
     </row>
     <row r="188">
-      <c r="A188" t="n">
-        <v>0</v>
+      <c r="A188" t="inlineStr">
+        <is>
+          <t>Koordinasi, Kapolsek, Koramil, Sugiarto, Iptu Sri Windiarto, Longsor</t>
+        </is>
       </c>
       <c r="B188" t="n">
         <v>0</v>
@@ -24411,8 +24785,10 @@
       </c>
     </row>
     <row r="189">
-      <c r="A189" t="n">
-        <v>0</v>
+      <c r="A189" t="inlineStr">
+        <is>
+          <t>Pasar, Sandi, PMK</t>
+        </is>
       </c>
       <c r="B189" t="n">
         <v>0</v>
@@ -24525,8 +24901,10 @@
       </c>
     </row>
     <row r="190">
-      <c r="A190" t="n">
-        <v>0</v>
+      <c r="A190" t="inlineStr">
+        <is>
+          <t>Lengser, Arab Saudi, Gedung Juang, Sunda, Ambu, Klasmi, Penyelenggara Yudi Onyeh, Komunitas Forum Film, Yudi, Komunitas Soeraoeng Komedi</t>
+        </is>
       </c>
       <c r="B190" t="n">
         <v>0</v>
@@ -24671,8 +25049,10 @@
       </c>
     </row>
     <row r="191">
-      <c r="A191" t="n">
-        <v>0</v>
+      <c r="A191" t="inlineStr">
+        <is>
+          <t>BPBD, Polsek, Iptu Hartono, Hartono, Pasar, Polres, Mobil, Kapolsek, Kebakaran Pasar</t>
+        </is>
       </c>
       <c r="B191" t="n">
         <v>0</v>
@@ -24785,8 +25165,10 @@
       </c>
     </row>
     <row r="192">
-      <c r="A192" t="n">
-        <v>0</v>
+      <c r="A192" t="inlineStr">
+        <is>
+          <t>BPBD, Pos Krukut Hulu, Kali Lenggong, Meruya, Kali Krukut, DKI, Isnawa, BPBD DKI, Dukuh, Samala, Isnawa Adji, Pelaksana BPBD DKI, Kel, Pos Sunter Hulu</t>
+        </is>
       </c>
       <c r="B192" t="n">
         <v>0</v>
@@ -24918,8 +25300,10 @@
       </c>
     </row>
     <row r="193">
-      <c r="A193" t="n">
-        <v>0</v>
+      <c r="A193" t="inlineStr">
+        <is>
+          <t>Hadi, Pantai Batukaras, Batukaras, DetikJabar, Kepala, Batukaras Hadi Somantri</t>
+        </is>
       </c>
       <c r="B193" t="n">
         <v>0</v>
@@ -25043,8 +25427,10 @@
       </c>
     </row>
     <row r="194">
-      <c r="A194" t="n">
-        <v>0</v>
+      <c r="A194" t="inlineStr">
+        <is>
+          <t>Waduk, Wilayah, Pangkep, Hendra, Pelaksana BPBD Achmad Hendra Hakamuddin, Pompengan Jeneberang, BMKG, Posko Induk BBWS Pompengan Jeneberang</t>
+        </is>
       </c>
       <c r="B194" t="n">
         <v>0</v>
@@ -25181,8 +25567,10 @@
       </c>
     </row>
     <row r="195">
-      <c r="A195" t="n">
-        <v>0</v>
+      <c r="A195" t="inlineStr">
+        <is>
+          <t>BPBD, Kapolres Anambas AKBP Syafrudin Semidang, M Hasbi, Hasbi, Dinas Perindag, Anambas, Kepulauan, Disperindag, TNI, Kepri, BPBD Anambas</t>
+        </is>
       </c>
       <c r="B195" t="n">
         <v>0</v>
@@ -25302,8 +25690,10 @@
       </c>
     </row>
     <row r="196">
-      <c r="A196" t="n">
-        <v>0</v>
+      <c r="A196" t="inlineStr">
+        <is>
+          <t>Seksi Perawatan Lebah Kelompok Lebah Madu Buana Sari, Sukayana, Kelompok Tani Lebah Madu Buana Sari, Royal Jelly, Australia, Yehsumbul, Samblong</t>
+        </is>
       </c>
       <c r="B196" t="n">
         <v>0</v>
@@ -25430,8 +25820,10 @@
       </c>
     </row>
     <row r="197">
-      <c r="A197" t="n">
-        <v>0</v>
+      <c r="A197" t="inlineStr">
+        <is>
+          <t>Sabhara Polda, Pantauan, Brimob, Polres, Eko, Erina, SOP</t>
+        </is>
       </c>
       <c r="B197" t="n">
         <v>0</v>
@@ -25479,12 +25871,12 @@
       </c>
       <c r="N197" t="inlineStr">
         <is>
-          <t>bandung</t>
+          <t>klaten</t>
         </is>
       </c>
       <c r="O197" t="inlineStr">
         <is>
-          <t>jawa barat</t>
+          <t>jawa tengah</t>
         </is>
       </c>
       <c r="P197" t="n">
@@ -25552,8 +25944,10 @@
       </c>
     </row>
     <row r="198">
-      <c r="A198" t="n">
-        <v>0</v>
+      <c r="A198" t="inlineStr">
+        <is>
+          <t>Deborah Juliani, UMKM, Deborah</t>
+        </is>
       </c>
       <c r="B198" t="n">
         <v>0</v>
@@ -25670,8 +26064,10 @@
       </c>
     </row>
     <row r="199">
-      <c r="A199" t="n">
-        <v>0</v>
+      <c r="A199" t="inlineStr">
+        <is>
+          <t>Atik, Mampang, Kompas TV</t>
+        </is>
       </c>
       <c r="B199" t="n">
         <v>0</v>
@@ -25719,12 +26115,12 @@
       </c>
       <c r="N199" t="inlineStr">
         <is>
-          <t>bangka</t>
+          <t>jakarta selatan</t>
         </is>
       </c>
       <c r="O199" t="inlineStr">
         <is>
-          <t>bangka belitung</t>
+          <t>dki jakarta</t>
         </is>
       </c>
       <c r="P199" t="n">
@@ -25775,8 +26171,10 @@
       </c>
     </row>
     <row r="200">
-      <c r="A200" t="n">
-        <v>0</v>
+      <c r="A200" t="inlineStr">
+        <is>
+          <t>Tana Toraja, Kepala BPBD Tana Toraja Christian Batara Sakkung, Poros, Gregorius Feri, BPBD Tana Toraja, Dinsos Tana Toraja, Gregorius</t>
+        </is>
       </c>
       <c r="B200" t="n">
         <v>0</v>
@@ -25895,8 +26293,10 @@
       </c>
     </row>
     <row r="201">
-      <c r="A201" t="n">
-        <v>0</v>
+      <c r="A201" t="inlineStr">
+        <is>
+          <t>Kristiani, Sti Nenotek, Stasiun Meteorologi</t>
+        </is>
       </c>
       <c r="B201" t="n">
         <v>0</v>
@@ -26008,8 +26408,10 @@
       </c>
     </row>
     <row r="202">
-      <c r="A202" t="n">
-        <v>0</v>
+      <c r="A202" t="inlineStr">
+        <is>
+          <t>Matahari, Andi, Riset Antariksa BRIN Andi Pangerang, Solstis, Edukasi Sains BRIN, Bumi</t>
+        </is>
       </c>
       <c r="B202" t="n">
         <v>0</v>
@@ -26131,8 +26533,10 @@
       </c>
     </row>
     <row r="203">
-      <c r="A203" t="n">
-        <v>0</v>
+      <c r="A203" t="inlineStr">
+        <is>
+          <t>Badan Meteorologi, Klimatologi, BMKG, NTB</t>
+        </is>
       </c>
       <c r="B203" t="n">
         <v>0</v>
@@ -26249,8 +26653,10 @@
       </c>
     </row>
     <row r="204">
-      <c r="A204" t="n">
-        <v>0</v>
+      <c r="A204" t="inlineStr">
+        <is>
+          <t>Halu Oleo, BBKSDA, Oh, Cimekar, Halu</t>
+        </is>
       </c>
       <c r="B204" t="n">
         <v>0</v>
@@ -26399,8 +26805,10 @@
       </c>
     </row>
     <row r="205">
-      <c r="A205" t="n">
-        <v>0</v>
+      <c r="A205" t="inlineStr">
+        <is>
+          <t>Antara, Akmal, Gubernur, Pemerintah, Tampalang</t>
+        </is>
       </c>
       <c r="B205" t="n">
         <v>0</v>
@@ -26522,8 +26930,10 @@
       </c>
     </row>
     <row r="206">
-      <c r="A206" t="n">
-        <v>0</v>
+      <c r="A206" t="inlineStr">
+        <is>
+          <t>DOK, Humas Dompet Dhuafa Erika, Tuhan, SAR DMC Dompet Dhuafa, Indonesia, Dompet Dhuafa, Erika</t>
+        </is>
       </c>
       <c r="B206" t="n">
         <v>0</v>
@@ -26571,7 +26981,7 @@
       </c>
       <c r="N206" t="inlineStr">
         <is>
-          <t>bandung</t>
+          <t>cianjur</t>
         </is>
       </c>
       <c r="O206" t="inlineStr">
@@ -26677,8 +27087,10 @@
       </c>
     </row>
     <row r="207">
-      <c r="A207" t="n">
-        <v>0</v>
+      <c r="A207" t="inlineStr">
+        <is>
+          <t>BPBD, Gatot, Gatot Soebroto, Kalaksa BPBD, Madura, Bu Gubernur, BMKG</t>
+        </is>
       </c>
       <c r="B207" t="n">
         <v>0</v>
@@ -26798,8 +27210,10 @@
       </c>
     </row>
     <row r="208">
-      <c r="A208" t="n">
-        <v>0</v>
+      <c r="A208" t="inlineStr">
+        <is>
+          <t>Asep, Asep Hendradiana, IGD, Kapusdokkes Polri Irjen, Polri, RS Bhayangkara Setukpa</t>
+        </is>
       </c>
       <c r="B208" t="n">
         <v>0</v>
@@ -26929,8 +27343,10 @@
       </c>
     </row>
     <row r="209">
-      <c r="A209" t="n">
-        <v>0</v>
+      <c r="A209" t="inlineStr">
+        <is>
+          <t>Badan Pertanahan Nasional, Edy, Simeme, Bupati Deli Serdang Ashari Tambunan, Edy Rahmayadi, Kepulauan, Dilansir</t>
+        </is>
       </c>
       <c r="B209" t="n">
         <v>0</v>

</xml_diff>